<commit_message>
diveded into a file, but not fixed bags and style
</commit_message>
<xml_diff>
--- a/data/result с верными входными данными.xlsx
+++ b/data/result с верными входными данными.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\OneDrive - riverw\ДАША\Другое\альтернативный код проект\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://riverw-my.sharepoint.com/personal/7963_365hub_club/Documents/ДАША/Другое/альтернативный код проект/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390050B8-D583-4EE9-BA45-9A79754A67F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{390050B8-D583-4EE9-BA45-9A79754A67F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A01EA8F6-B2FE-4F07-A009-478EF9CE4D1F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{313C0AA6-9A72-4474-91A1-AFEFE7A83AF4}"/>
   </bookViews>
@@ -63,13 +63,13 @@
     <t>ошибка робастного метода maxiter=5</t>
   </si>
   <si>
-    <t>Здесь точность 0.0001</t>
+    <t>Кросс валидация робаста maxiter=50</t>
   </si>
   <si>
-    <t>тут ошибка 0.01</t>
+    <t>eps 0.0001</t>
   </si>
   <si>
-    <t>Кросс валидация робаста maxiter=50</t>
+    <t xml:space="preserve"> eps  0.01</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L23" sqref="I23:L23"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1572,12 +1572,12 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="1"/>
       <c r="E32" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
do some research with emissions
</commit_message>
<xml_diff>
--- a/data/result с верными входными данными.xlsx
+++ b/data/result с верными входными данными.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\voronkina.2018\Desktop\проектная деятельность\BioProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://riverw-my.sharepoint.com/personal/7963_365hub_club/Documents/ДАША/Другое/альтернативный код проект/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_43AB77CB8C22618027FAA901E6906528479AF978" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7CBF03D8-7463-4728-841B-7D619D1F0EEF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="4" r:id="rId1"/>
@@ -18,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -83,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,7 +150,7 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="3"/>
+    <cellStyle name="Обычный 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Плохой" xfId="2" builtinId="27"/>
     <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -471,11 +463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +480,7 @@
     <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="40.5703125" bestFit="1" customWidth="1"/>

</xml_diff>